<commit_message>
weight of craft weapons and missiles was checked
</commit_message>
<xml_diff>
--- a/WorkFiles/CraftWeapons.xlsx
+++ b/WorkFiles/CraftWeapons.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Weapon</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Sell</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>x50</t>
+  </si>
+  <si>
+    <t>x40</t>
   </si>
 </sst>
 </file>
@@ -152,7 +161,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="YYYY/MM/DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -173,11 +182,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -206,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -243,6 +247,20 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="hair"/>
@@ -252,6 +270,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
@@ -282,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,10 +364,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,14 +384,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,7 +416,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,7 +432,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,16 +440,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -511,7 +552,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -521,7 +562,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.2857142857143"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="11.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.5459183673469"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.94897959183674"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.3214285714286"/>
@@ -647,11 +688,11 @@
         <f aca="false">G3*C3</f>
         <v>360</v>
       </c>
-      <c r="I3" s="14" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">C3*K3</f>
         <v>60</v>
       </c>
-      <c r="J3" s="15" t="n">
+      <c r="J3" s="14" t="n">
         <f aca="false">C3/F3*D3/100</f>
         <v>0.5</v>
       </c>
@@ -667,49 +708,49 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+    <row r="4" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="n">
+      <c r="C4" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="20" t="n">
+      <c r="F4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="21" t="n">
+      <c r="G4" s="19" t="n">
         <v>100</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="16" t="n">
         <f aca="false">G4*C4</f>
         <v>1000</v>
       </c>
-      <c r="I4" s="22" t="n">
+      <c r="I4" s="19" t="n">
         <f aca="false">C4*K4</f>
         <v>160</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="20" t="n">
         <f aca="false">C4/F4*D4/100</f>
         <v>0.8</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="K4" s="21" t="n">
         <f aca="false">ROUND(G4/(G4/(D4*G4/100)),0)</f>
         <v>16</v>
       </c>
-      <c r="L4" s="24" t="n">
+      <c r="L4" s="21" t="n">
         <f aca="false">F4*G4</f>
         <v>200</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -785,11 +826,11 @@
         <f aca="false">G6*C6</f>
         <v>360</v>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="1" t="n">
         <f aca="false">C6*K6</f>
         <v>240</v>
       </c>
-      <c r="J6" s="15" t="n">
+      <c r="J6" s="14" t="n">
         <f aca="false">C6/F6*D6/100</f>
         <v>2</v>
       </c>
@@ -805,49 +846,49 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+    <row r="7" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="17" t="n">
+      <c r="B7" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C7" s="17" t="n">
+      <c r="C7" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="20" t="n">
+      <c r="F7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="21" t="n">
+      <c r="G7" s="19" t="n">
         <v>120</v>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="16" t="n">
         <f aca="false">G7*C7</f>
         <v>1200</v>
       </c>
-      <c r="I7" s="22" t="n">
+      <c r="I7" s="19" t="n">
         <f aca="false">C7*K7</f>
         <v>580</v>
       </c>
-      <c r="J7" s="23" t="n">
+      <c r="J7" s="20" t="n">
         <f aca="false">C7/F7*D7/100</f>
         <v>2.4</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="21" t="n">
         <f aca="false">ROUND(G7/(G7/(D7*G7/100)),0)</f>
         <v>58</v>
       </c>
-      <c r="L7" s="24" t="n">
+      <c r="L7" s="21" t="n">
         <f aca="false">F7*G7</f>
         <v>240</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -877,11 +918,11 @@
         <f aca="false">G8*C8</f>
         <v>1680</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="1" t="n">
         <f aca="false">C8*K8</f>
         <v>804</v>
       </c>
-      <c r="J8" s="15" t="n">
+      <c r="J8" s="14" t="n">
         <f aca="false">C8/F8*D8/100</f>
         <v>1.44</v>
       </c>
@@ -923,11 +964,11 @@
         <f aca="false">G9*C9</f>
         <v>960</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="1" t="n">
         <f aca="false">C9*K9</f>
         <v>780</v>
       </c>
-      <c r="J9" s="15" t="n">
+      <c r="J9" s="14" t="n">
         <f aca="false">C9/F9*D9/100</f>
         <v>2</v>
       </c>
@@ -943,37 +984,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+    <row r="10" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="17" t="n">
+      <c r="B10" s="16" t="n">
         <v>36</v>
       </c>
-      <c r="C10" s="17" t="n">
+      <c r="C10" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="26" t="n">
+      <c r="F10" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="G10" s="21" t="n">
+      <c r="G10" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="H10" s="17" t="n">
+      <c r="H10" s="16" t="n">
         <f aca="false">G10*C10</f>
         <v>1200</v>
       </c>
-      <c r="I10" s="22" t="n">
+      <c r="I10" s="19" t="n">
         <f aca="false">C10*K10</f>
         <v>675</v>
       </c>
-      <c r="J10" s="15" t="n">
+      <c r="J10" s="14" t="n">
         <f aca="false">C10/F10*D10/100</f>
         <v>2.75</v>
       </c>
@@ -985,53 +1026,53 @@
         <f aca="false">F10*G10</f>
         <v>240</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="17" t="n">
+      <c r="B11" s="16" t="n">
         <v>65</v>
       </c>
-      <c r="C11" s="17" t="n">
+      <c r="C11" s="16" t="n">
         <v>310</v>
       </c>
-      <c r="D11" s="18" t="n">
+      <c r="D11" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="26" t="n">
+      <c r="F11" s="23" t="n">
         <v>28</v>
       </c>
-      <c r="G11" s="27" t="n">
+      <c r="G11" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="17" t="n">
+      <c r="H11" s="16" t="n">
         <f aca="false">G11*C11</f>
         <v>620</v>
       </c>
-      <c r="I11" s="27" t="n">
+      <c r="I11" s="24" t="n">
         <f aca="false">C11*K11</f>
         <v>620</v>
       </c>
-      <c r="J11" s="28" t="n">
+      <c r="J11" s="25" t="n">
         <f aca="false">C11/F11*D11/100</f>
         <v>10.5178571428571</v>
       </c>
-      <c r="K11" s="29" t="n">
+      <c r="K11" s="26" t="n">
         <f aca="false">ROUND(G11/(G11/(D11*G11/100)),0)</f>
         <v>2</v>
       </c>
-      <c r="L11" s="29" t="n">
+      <c r="L11" s="26" t="n">
         <f aca="false">F11*G11</f>
         <v>56</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="M11" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1048,19 +1089,25 @@
       <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
+      <c r="I14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
@@ -1072,10 +1119,19 @@
       <c r="D15" s="1" t="n">
         <v>63750</v>
       </c>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
+      <c r="E15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>11250</v>
+      </c>
       <c r="G15" s="0"/>
-      <c r="I15" s="0"/>
+      <c r="H15" s="0" t="n">
+        <v>8500</v>
+      </c>
+      <c r="I15" s="28" t="n">
+        <v>1.2</v>
+      </c>
       <c r="J15" s="0"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1090,41 +1146,67 @@
       <c r="D16" s="1" t="n">
         <v>8500</v>
       </c>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
+      <c r="E16" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>3000</v>
+      </c>
       <c r="G16" s="0"/>
-      <c r="I16" s="0"/>
+      <c r="H16" s="0" t="n">
+        <v>2400</v>
+      </c>
+      <c r="I16" s="28" t="n">
+        <v>0.4</v>
+      </c>
       <c r="J16" s="0"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
+    <row r="17" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="17" t="n">
+      <c r="B17" s="16" t="n">
         <v>16000</v>
       </c>
-      <c r="D17" s="21" t="n">
+      <c r="D17" s="19" t="n">
         <v>12000</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
+      <c r="E17" s="19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="16" t="n">
+        <v>1240</v>
+      </c>
+      <c r="H17" s="16" t="n">
+        <v>1012</v>
+      </c>
+      <c r="I17" s="29" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="31" t="n">
+      <c r="C18" s="30" t="n">
         <v>31875</v>
       </c>
-      <c r="D18" s="32" t="n">
+      <c r="D18" s="31" t="n">
         <v>76500</v>
       </c>
-      <c r="E18" s="0"/>
+      <c r="E18" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
-      <c r="I18" s="0"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="0"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1133,33 +1215,38 @@
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="31" t="n">
+      <c r="C19" s="30" t="n">
         <v>4250</v>
       </c>
-      <c r="D19" s="32" t="n">
+      <c r="D19" s="31" t="n">
         <v>10200</v>
       </c>
-      <c r="E19" s="0"/>
+      <c r="E19" s="1" t="n">
+        <v>0.8</v>
+      </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
-      <c r="I19" s="0"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="0"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+    <row r="20" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="33" t="n">
+      <c r="C20" s="32" t="n">
         <v>6000</v>
       </c>
-      <c r="D20" s="34" t="n">
+      <c r="D20" s="33" t="n">
         <v>14400</v>
       </c>
-      <c r="E20" s="0"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
+      <c r="E20" s="19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I20" s="29"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
@@ -1171,15 +1258,22 @@
       <c r="D21" s="1" t="n">
         <v>204000</v>
       </c>
-      <c r="E21" s="35" t="n">
+      <c r="E21" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H21" s="34" t="n">
         <v>3500</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G21" s="0"/>
-      <c r="I21" s="0"/>
-      <c r="J21" s="0"/>
+      <c r="I21" s="28" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
@@ -1193,41 +1287,60 @@
       <c r="D22" s="1" t="n">
         <v>211000</v>
       </c>
-      <c r="E22" s="0"/>
+      <c r="E22" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
-      <c r="I22" s="0"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="0"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+    <row r="23" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="17" t="n">
+      <c r="C23" s="16" t="n">
         <v>226000</v>
       </c>
-      <c r="D23" s="21" t="n">
+      <c r="D23" s="19" t="n">
         <v>267300</v>
       </c>
-      <c r="E23" s="0"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
+      <c r="E23" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="I23" s="29"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="17" t="n">
+      <c r="C24" s="36" t="n">
         <v>242000</v>
       </c>
-      <c r="D24" s="21" t="n">
+      <c r="D24" s="37" t="n">
         <v>281000</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
+      <c r="E24" s="37" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G24" s="38" t="n">
+        <v>28000</v>
+      </c>
+      <c r="H24" s="36" t="n">
+        <v>53300</v>
+      </c>
+      <c r="I24" s="39" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J24" s="37"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
LASER and PLASMA craft weapon improvment
</commit_message>
<xml_diff>
--- a/WorkFiles/CraftWeapons.xlsx
+++ b/WorkFiles/CraftWeapons.xlsx
@@ -113,7 +113,7 @@
     <t>LASER CANNON</t>
   </si>
   <si>
-    <t>13/12/11</t>
+    <t>10-10-10</t>
   </si>
   <si>
     <t>PLASMA BEAM</t>
@@ -122,7 +122,7 @@
     <t>55</t>
   </si>
   <si>
-    <t>16/15/14</t>
+    <t>11/11/11</t>
   </si>
   <si>
     <t>FUSION BALL</t>
@@ -307,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,6 +398,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -551,8 +555,8 @@
   </sheetPr>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -951,11 +955,11 @@
       <c r="D9" s="9" t="n">
         <v>80</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>32</v>
@@ -970,7 +974,7 @@
       </c>
       <c r="J9" s="14" t="n">
         <f aca="false">C9/F9*D9/100</f>
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="K9" s="12" t="n">
         <f aca="false">ROUND(G9/(G9/(D9*G9/100)),0)</f>
@@ -978,7 +982,7 @@
       </c>
       <c r="L9" s="12" t="n">
         <f aca="false">F9*G9</f>
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="M9" s="13" t="s">
         <v>31</v>
@@ -997,11 +1001,11 @@
       <c r="D10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="23" t="n">
-        <v>15</v>
+      <c r="F10" s="24" t="n">
+        <v>11</v>
       </c>
       <c r="G10" s="19" t="n">
         <v>16</v>
@@ -1016,7 +1020,7 @@
       </c>
       <c r="J10" s="14" t="n">
         <f aca="false">C10/F10*D10/100</f>
-        <v>2.75</v>
+        <v>3.75</v>
       </c>
       <c r="K10" s="12" t="n">
         <f aca="false">ROUND(G10/(G10/(D10*G10/100)),0)</f>
@@ -1024,7 +1028,7 @@
       </c>
       <c r="L10" s="12" t="n">
         <f aca="false">F10*G10</f>
-        <v>240</v>
+        <v>176</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>33</v>
@@ -1043,32 +1047,32 @@
       <c r="D11" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="23" t="n">
+      <c r="F11" s="24" t="n">
         <v>28</v>
       </c>
-      <c r="G11" s="24" t="n">
+      <c r="G11" s="25" t="n">
         <v>2</v>
       </c>
       <c r="H11" s="16" t="n">
         <f aca="false">G11*C11</f>
         <v>620</v>
       </c>
-      <c r="I11" s="24" t="n">
+      <c r="I11" s="25" t="n">
         <f aca="false">C11*K11</f>
         <v>620</v>
       </c>
-      <c r="J11" s="25" t="n">
+      <c r="J11" s="26" t="n">
         <f aca="false">C11/F11*D11/100</f>
         <v>10.5178571428571</v>
       </c>
-      <c r="K11" s="26" t="n">
+      <c r="K11" s="27" t="n">
         <f aca="false">ROUND(G11/(G11/(D11*G11/100)),0)</f>
         <v>2</v>
       </c>
-      <c r="L11" s="26" t="n">
+      <c r="L11" s="27" t="n">
         <f aca="false">F11*G11</f>
         <v>56</v>
       </c>
@@ -1104,10 +1108,10 @@
       <c r="I14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
@@ -1129,7 +1133,7 @@
       <c r="H15" s="0" t="n">
         <v>8500</v>
       </c>
-      <c r="I15" s="28" t="n">
+      <c r="I15" s="29" t="n">
         <v>1.2</v>
       </c>
       <c r="J15" s="0"/>
@@ -1156,7 +1160,7 @@
       <c r="H16" s="0" t="n">
         <v>2400</v>
       </c>
-      <c r="I16" s="28" t="n">
+      <c r="I16" s="29" t="n">
         <v>0.4</v>
       </c>
       <c r="J16" s="0"/>
@@ -1182,23 +1186,23 @@
       <c r="H17" s="16" t="n">
         <v>1012</v>
       </c>
-      <c r="I17" s="29" t="n">
+      <c r="I17" s="30" t="n">
         <v>0.1</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="30" t="n">
+      <c r="C18" s="31" t="n">
         <v>31875</v>
       </c>
-      <c r="D18" s="31" t="n">
+      <c r="D18" s="32" t="n">
         <v>76500</v>
       </c>
       <c r="E18" s="1" t="n">
@@ -1206,7 +1210,7 @@
       </c>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
-      <c r="I18" s="28"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="0"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1215,10 +1219,10 @@
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="30" t="n">
+      <c r="C19" s="31" t="n">
         <v>4250</v>
       </c>
-      <c r="D19" s="31" t="n">
+      <c r="D19" s="32" t="n">
         <v>10200</v>
       </c>
       <c r="E19" s="1" t="n">
@@ -1226,7 +1230,7 @@
       </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
-      <c r="I19" s="28"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="0"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1235,18 +1239,18 @@
       <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="32" t="n">
+      <c r="C20" s="33" t="n">
         <v>6000</v>
       </c>
-      <c r="D20" s="33" t="n">
+      <c r="D20" s="34" t="n">
         <v>14400</v>
       </c>
       <c r="E20" s="19" t="n">
         <v>1.5</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
+      <c r="I20" s="30"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
@@ -1261,14 +1265,14 @@
       <c r="E21" s="1" t="n">
         <v>2.4</v>
       </c>
-      <c r="F21" s="34"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="H21" s="34" t="n">
+      <c r="H21" s="35" t="n">
         <v>3500</v>
       </c>
-      <c r="I21" s="28" t="n">
+      <c r="I21" s="29" t="n">
         <v>0.1</v>
       </c>
       <c r="J21" s="0" t="s">
@@ -1292,7 +1296,7 @@
       </c>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
-      <c r="I22" s="28"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="0"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1312,35 +1316,35 @@
       </c>
       <c r="F23" s="0"/>
       <c r="H23" s="0"/>
-      <c r="I23" s="29"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
+      <c r="I23" s="30"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="36" t="n">
+      <c r="C24" s="37" t="n">
         <v>242000</v>
       </c>
-      <c r="D24" s="37" t="n">
+      <c r="D24" s="38" t="n">
         <v>281000</v>
       </c>
-      <c r="E24" s="37" t="n">
+      <c r="E24" s="38" t="n">
         <v>1.8</v>
       </c>
-      <c r="G24" s="38" t="n">
+      <c r="G24" s="39" t="n">
         <v>28000</v>
       </c>
-      <c r="H24" s="36" t="n">
+      <c r="H24" s="37" t="n">
         <v>53300</v>
       </c>
-      <c r="I24" s="39" t="n">
+      <c r="I24" s="40" t="n">
         <v>1.5</v>
       </c>
-      <c r="J24" s="37"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>